<commit_message>
routine analysis update + few minor fixes in excel mngmt
</commit_message>
<xml_diff>
--- a/default/data/Clean/NCASH.xlsx
+++ b/default/data/Clean/NCASH.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="64">
   <si>
     <t>Cash_N500</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>AMBER.NS</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>VIPIND.NS</t>
+  </si>
+  <si>
+    <t>SJVN.NS</t>
+  </si>
+  <si>
+    <t>RHIM.NS</t>
+  </si>
+  <si>
+    <t>JSL.NS</t>
+  </si>
+  <si>
+    <t>THERMAX.NS</t>
   </si>
 </sst>
 </file>
@@ -554,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,40 +639,40 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>44539</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2228.5</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2108.85</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1997.53</v>
-      </c>
-      <c r="H2" s="4">
-        <v>2295.36</v>
-      </c>
-      <c r="I2" s="4">
-        <v>2360.58</v>
-      </c>
-      <c r="J2" s="4">
-        <v>2638.53</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="4">
-        <v>2244.5500000000002</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>4</v>
+        <v>44575</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>499.65</v>
+      </c>
+      <c r="F2">
+        <v>468.25</v>
+      </c>
+      <c r="G2">
+        <v>464.03</v>
+      </c>
+      <c r="H2">
+        <v>514.64</v>
+      </c>
+      <c r="I2">
+        <v>515.6</v>
+      </c>
+      <c r="J2">
+        <v>529.22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2">
+        <v>504.2</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -665,40 +683,40 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>44533</v>
+        <v>44573</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="E3">
-        <v>364.15</v>
+        <v>596.4</v>
       </c>
       <c r="F3">
-        <v>337.79</v>
+        <v>568.29</v>
       </c>
       <c r="G3">
-        <v>318.74</v>
+        <v>551.22</v>
       </c>
       <c r="H3">
-        <v>375.07</v>
+        <v>614.29</v>
       </c>
       <c r="I3">
-        <v>385.52</v>
+        <v>669</v>
       </c>
       <c r="J3">
-        <v>403.45</v>
+        <v>780.4</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="L3">
-        <v>421.05</v>
+        <v>588.15</v>
       </c>
       <c r="M3">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -709,40 +727,40 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>44533</v>
+        <v>44571</v>
       </c>
       <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>31.8</v>
+      </c>
+      <c r="F4">
+        <v>29.37</v>
+      </c>
+      <c r="G4">
+        <v>28.98</v>
+      </c>
+      <c r="H4">
+        <v>32.75</v>
+      </c>
+      <c r="I4">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="J4">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4">
+        <v>31.35</v>
+      </c>
+      <c r="M4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>154.94999999999999</v>
-      </c>
-      <c r="F4">
-        <v>151.22</v>
-      </c>
-      <c r="G4">
-        <v>147.36000000000001</v>
-      </c>
-      <c r="H4">
-        <v>159.6</v>
-      </c>
-      <c r="I4">
-        <v>160.97999999999999</v>
-      </c>
-      <c r="J4">
-        <v>167.95</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <v>146.05000000000001</v>
-      </c>
-      <c r="M4">
-        <v>3</v>
-      </c>
       <c r="N4" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -753,34 +771,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>44531</v>
+        <v>44571</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E5">
-        <v>5080.25</v>
+        <v>382.05</v>
       </c>
       <c r="F5">
-        <v>4957.96</v>
+        <v>367</v>
       </c>
       <c r="G5">
-        <v>4845.8599999999997</v>
+        <v>356.22</v>
       </c>
       <c r="H5">
-        <v>5220.53</v>
+        <v>391.12</v>
       </c>
       <c r="I5">
-        <v>5232.66</v>
+        <v>393.51</v>
       </c>
       <c r="J5">
-        <v>5311.9</v>
+        <v>403.35</v>
       </c>
       <c r="K5" t="s">
         <v>3</v>
       </c>
       <c r="L5">
-        <v>5060.1000000000004</v>
+        <v>421</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -797,37 +815,37 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>44526</v>
+        <v>44568</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>1810.1</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="F6">
-        <v>1745.93</v>
+        <v>147.59</v>
       </c>
       <c r="G6">
-        <v>1715.01</v>
+        <v>147.49</v>
       </c>
       <c r="H6">
-        <v>1864.4</v>
+        <v>163.46</v>
       </c>
       <c r="I6">
-        <v>1887.2</v>
+        <v>166.75</v>
       </c>
       <c r="J6">
-        <v>2088.1999999999998</v>
+        <v>184.75</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <v>1974.55</v>
+        <v>176.2</v>
       </c>
       <c r="M6">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N6" t="s">
         <v>4</v>
@@ -841,37 +859,37 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>44522</v>
+        <v>44568</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="E7">
-        <v>142.9</v>
+        <v>200.65</v>
       </c>
       <c r="F7">
-        <v>133.26</v>
+        <v>190.7</v>
       </c>
       <c r="G7">
-        <v>127.28</v>
+        <v>183.28</v>
       </c>
       <c r="H7">
-        <v>147.19</v>
+        <v>206.67</v>
       </c>
       <c r="I7">
-        <v>149.35</v>
+        <v>214.8</v>
       </c>
       <c r="J7">
-        <v>156.41999999999999</v>
+        <v>223.1</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="L7">
-        <v>149.30000000000001</v>
+        <v>204.65</v>
       </c>
       <c r="M7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N7" t="s">
         <v>4</v>
@@ -885,40 +903,40 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>44517</v>
+        <v>44566</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="E8">
-        <v>230.3</v>
+        <v>1903.9</v>
       </c>
       <c r="F8">
-        <v>218.03</v>
+        <v>1755.34</v>
       </c>
       <c r="G8">
-        <v>214.41</v>
+        <v>1642.64</v>
       </c>
       <c r="H8">
-        <v>237.21</v>
+        <v>1961.02</v>
       </c>
       <c r="I8">
-        <v>241.3</v>
+        <v>1969.95</v>
       </c>
       <c r="J8">
-        <v>258</v>
+        <v>2061.4699999999998</v>
       </c>
       <c r="K8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>213.5</v>
+        <v>2068.0500000000002</v>
       </c>
       <c r="M8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -929,40 +947,40 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>44516</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>504</v>
-      </c>
-      <c r="F9">
-        <v>485.12</v>
-      </c>
-      <c r="G9">
-        <v>474.56</v>
-      </c>
-      <c r="H9">
-        <v>519.12</v>
-      </c>
-      <c r="I9">
-        <v>564.98</v>
-      </c>
-      <c r="J9">
-        <v>657.23</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <v>425.5</v>
-      </c>
-      <c r="M9">
-        <v>4</v>
-      </c>
-      <c r="N9" t="s">
-        <v>6</v>
+        <v>44539</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2228.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2108.85</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1997.53</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2295.36</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2360.58</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2638.53</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2244.5500000000002</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -973,40 +991,40 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>44516</v>
+        <v>44533</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>2288.75</v>
+        <v>364.15</v>
       </c>
       <c r="F10">
-        <v>2194.21</v>
+        <v>337.79</v>
       </c>
       <c r="G10">
-        <v>2184.1799999999998</v>
+        <v>318.74</v>
       </c>
       <c r="H10">
-        <v>2357.41</v>
+        <v>375.07</v>
       </c>
       <c r="I10">
-        <v>2392.4499999999998</v>
+        <v>385.52</v>
       </c>
       <c r="J10">
-        <v>2609.85</v>
+        <v>403.45</v>
       </c>
       <c r="K10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>1911.7</v>
+        <v>421.05</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1017,37 +1035,37 @@
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>44515</v>
+        <v>44533</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>367.8</v>
+        <v>154.94999999999999</v>
       </c>
       <c r="F11">
-        <v>356.44</v>
+        <v>151.22</v>
       </c>
       <c r="G11">
-        <v>341.13</v>
+        <v>147.36000000000001</v>
       </c>
       <c r="H11">
-        <v>378.83</v>
+        <v>159.6</v>
       </c>
       <c r="I11">
-        <v>387.22</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="J11">
-        <v>433.87</v>
+        <v>167.95</v>
       </c>
       <c r="K11" t="s">
         <v>6</v>
       </c>
       <c r="L11">
-        <v>374.15</v>
+        <v>146.05000000000001</v>
       </c>
       <c r="M11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N11" t="s">
         <v>6</v>
@@ -1061,37 +1079,37 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>44515</v>
+        <v>44531</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>926.25</v>
+        <v>5080.25</v>
       </c>
       <c r="F12">
-        <v>869.94</v>
+        <v>4957.96</v>
       </c>
       <c r="G12">
-        <v>866.86</v>
+        <v>4845.8599999999997</v>
       </c>
       <c r="H12">
-        <v>954.04</v>
+        <v>5220.53</v>
       </c>
       <c r="I12">
-        <v>959.1</v>
+        <v>5232.66</v>
       </c>
       <c r="J12">
-        <v>1056.0999999999999</v>
+        <v>5311.9</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L12">
-        <v>918.2</v>
+        <v>5060.1000000000004</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N12" t="s">
         <v>4</v>
@@ -1105,34 +1123,34 @@
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>44512</v>
+        <v>44526</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>922.15</v>
+        <v>1810.1</v>
       </c>
       <c r="F13">
-        <v>866.97</v>
+        <v>1745.93</v>
       </c>
       <c r="G13">
-        <v>846.17</v>
+        <v>1715.01</v>
       </c>
       <c r="H13">
-        <v>949.81</v>
+        <v>1864.4</v>
       </c>
       <c r="I13">
-        <v>959.97</v>
+        <v>1887.2</v>
       </c>
       <c r="J13">
-        <v>1104.8699999999999</v>
+        <v>2088.1999999999998</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="L13">
-        <v>925.35</v>
+        <v>1974.55</v>
       </c>
       <c r="M13">
         <v>14</v>
@@ -1149,40 +1167,40 @@
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>44512</v>
+        <v>44522</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>2252.3000000000002</v>
+        <v>142.9</v>
       </c>
       <c r="F14">
-        <v>2189.8000000000002</v>
+        <v>133.26</v>
       </c>
       <c r="G14">
-        <v>2179.61</v>
+        <v>127.28</v>
       </c>
       <c r="H14">
-        <v>2319.87</v>
+        <v>147.19</v>
       </c>
       <c r="I14">
-        <v>2392.4499999999998</v>
+        <v>149.35</v>
       </c>
       <c r="J14">
-        <v>2609.85</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="K14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>2042.05</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="M14">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1193,40 +1211,40 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>4169.55</v>
+        <v>230.3</v>
       </c>
       <c r="F15">
-        <v>4107.1499999999996</v>
+        <v>218.03</v>
       </c>
       <c r="G15">
-        <v>3788.59</v>
+        <v>214.41</v>
       </c>
       <c r="H15">
-        <v>4294.6400000000003</v>
+        <v>237.21</v>
       </c>
       <c r="I15">
-        <v>4574.22</v>
+        <v>241.3</v>
       </c>
       <c r="J15">
-        <v>4830.2700000000004</v>
+        <v>258</v>
       </c>
       <c r="K15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L15">
-        <v>3861.95</v>
+        <v>213.5</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1237,40 +1255,40 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>44509</v>
+        <v>44516</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E16">
-        <v>2006.35</v>
+        <v>504</v>
       </c>
       <c r="F16">
-        <v>1940.16</v>
+        <v>485.12</v>
       </c>
       <c r="G16">
-        <v>1849.85</v>
+        <v>474.56</v>
       </c>
       <c r="H16">
-        <v>2066.54</v>
+        <v>519.12</v>
       </c>
       <c r="I16">
-        <v>2111.6</v>
+        <v>564.98</v>
       </c>
       <c r="J16">
-        <v>2406.8000000000002</v>
+        <v>657.23</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L16">
-        <v>1966.85</v>
+        <v>425.5</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1281,37 +1299,37 @@
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>44504</v>
+        <v>44516</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <v>1438</v>
+        <v>2288.75</v>
       </c>
       <c r="F17">
-        <v>1348.05</v>
+        <v>2194.21</v>
       </c>
       <c r="G17">
-        <v>1246.52</v>
+        <v>2184.1799999999998</v>
       </c>
       <c r="H17">
-        <v>1481.14</v>
+        <v>2357.41</v>
       </c>
       <c r="I17">
-        <v>1500.53</v>
+        <v>2392.4499999999998</v>
       </c>
       <c r="J17">
-        <v>1557.03</v>
+        <v>2609.85</v>
       </c>
       <c r="K17" t="s">
         <v>6</v>
       </c>
       <c r="L17">
-        <v>1292.45</v>
+        <v>1911.7</v>
       </c>
       <c r="M17">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N17" t="s">
         <v>6</v>
@@ -1325,40 +1343,40 @@
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>44503</v>
+        <v>44515</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E18">
-        <v>940</v>
+        <v>367.8</v>
       </c>
       <c r="F18">
-        <v>889.59</v>
+        <v>356.44</v>
       </c>
       <c r="G18">
-        <v>877.45</v>
+        <v>341.13</v>
       </c>
       <c r="H18">
-        <v>968.2</v>
+        <v>378.83</v>
       </c>
       <c r="I18">
-        <v>976.45</v>
+        <v>387.22</v>
       </c>
       <c r="J18">
-        <v>1092.05</v>
+        <v>433.87</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L18">
-        <v>911.3</v>
+        <v>374.15</v>
       </c>
       <c r="M18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1369,37 +1387,37 @@
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>44503</v>
+        <v>44515</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>467.25</v>
+        <v>926.25</v>
       </c>
       <c r="F19">
-        <v>449.1</v>
+        <v>869.94</v>
       </c>
       <c r="G19">
-        <v>434.55</v>
+        <v>866.86</v>
       </c>
       <c r="H19">
-        <v>481.27</v>
+        <v>954.04</v>
       </c>
       <c r="I19">
-        <v>483.37</v>
+        <v>959.1</v>
       </c>
       <c r="J19">
-        <v>540.63</v>
+        <v>1056.0999999999999</v>
       </c>
       <c r="K19" t="s">
         <v>15</v>
       </c>
       <c r="L19">
-        <v>467.45</v>
+        <v>918.2</v>
       </c>
       <c r="M19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N19" t="s">
         <v>4</v>
@@ -1413,37 +1431,37 @@
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>44503</v>
+        <v>44512</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E20">
-        <v>2376.5500000000002</v>
+        <v>922.15</v>
       </c>
       <c r="F20">
-        <v>2227.59</v>
+        <v>866.97</v>
       </c>
       <c r="G20">
-        <v>2195.98</v>
+        <v>846.17</v>
       </c>
       <c r="H20">
-        <v>2447.7800000000002</v>
+        <v>949.81</v>
       </c>
       <c r="I20">
-        <v>2447.85</v>
+        <v>959.97</v>
       </c>
       <c r="J20">
-        <v>2581.4299999999998</v>
+        <v>1104.8699999999999</v>
       </c>
       <c r="K20" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="L20">
-        <v>2332.1</v>
+        <v>925.35</v>
       </c>
       <c r="M20">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N20" t="s">
         <v>4</v>
@@ -1457,40 +1475,40 @@
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>44503</v>
+        <v>44512</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>3960.1</v>
+        <v>2252.3000000000002</v>
       </c>
       <c r="F21">
-        <v>3811.12</v>
+        <v>2189.8000000000002</v>
       </c>
       <c r="G21">
-        <v>3778.9</v>
+        <v>2179.61</v>
       </c>
       <c r="H21">
-        <v>4078.9</v>
+        <v>2319.87</v>
       </c>
       <c r="I21">
-        <v>4094.88</v>
+        <v>2392.4499999999998</v>
       </c>
       <c r="J21">
-        <v>4611.7299999999996</v>
+        <v>2609.85</v>
       </c>
       <c r="K21" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L21">
-        <v>4220.7</v>
+        <v>2042.05</v>
       </c>
       <c r="M21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1501,40 +1519,40 @@
         <v>1</v>
       </c>
       <c r="C22" s="1">
-        <v>44502</v>
+        <v>44510</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E22">
-        <v>503</v>
+        <v>4169.55</v>
       </c>
       <c r="F22">
-        <v>468.45</v>
+        <v>4107.1499999999996</v>
       </c>
       <c r="G22">
-        <v>404.65</v>
+        <v>3788.59</v>
       </c>
       <c r="H22">
-        <v>518.09</v>
+        <v>4294.6400000000003</v>
       </c>
       <c r="I22">
-        <v>538.33000000000004</v>
+        <v>4574.22</v>
       </c>
       <c r="J22">
-        <v>564.23</v>
+        <v>4830.2700000000004</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L22">
-        <v>407.5</v>
+        <v>3861.95</v>
       </c>
       <c r="M22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1545,34 +1563,37 @@
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>44498</v>
+        <v>44509</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E23">
-        <v>183.95</v>
+        <v>2006.35</v>
       </c>
       <c r="F23">
-        <v>172.67</v>
+        <v>1940.16</v>
       </c>
       <c r="G23">
-        <v>150.44</v>
+        <v>1849.85</v>
       </c>
       <c r="H23">
-        <v>189.47</v>
+        <v>2066.54</v>
       </c>
       <c r="I23">
-        <v>220.63</v>
+        <v>2111.6</v>
+      </c>
+      <c r="J23">
+        <v>2406.8000000000002</v>
       </c>
       <c r="K23" t="s">
         <v>15</v>
       </c>
       <c r="L23">
-        <v>166.8</v>
+        <v>1966.85</v>
       </c>
       <c r="M23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N23" t="s">
         <v>4</v>
@@ -1586,40 +1607,40 @@
         <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>44497</v>
+        <v>44504</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E24">
-        <v>1947.1</v>
+        <v>1438</v>
       </c>
       <c r="F24">
-        <v>1858.11</v>
+        <v>1348.05</v>
       </c>
       <c r="G24">
-        <v>1845.66</v>
+        <v>1246.52</v>
       </c>
       <c r="H24">
-        <v>2005.51</v>
+        <v>1481.14</v>
       </c>
       <c r="I24">
-        <v>2022.07</v>
+        <v>1500.53</v>
       </c>
       <c r="J24">
-        <v>2175.9699999999998</v>
+        <v>1557.03</v>
       </c>
       <c r="K24" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L24">
-        <v>2149.5500000000002</v>
+        <v>1292.45</v>
       </c>
       <c r="M24">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1630,34 +1651,37 @@
         <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>44491</v>
+        <v>44503</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E25">
-        <v>50.1</v>
+        <v>940</v>
       </c>
       <c r="F25">
-        <v>46.38</v>
+        <v>889.59</v>
       </c>
       <c r="G25">
-        <v>45.6</v>
+        <v>877.45</v>
       </c>
       <c r="H25">
-        <v>52.35</v>
+        <v>968.2</v>
       </c>
       <c r="I25">
-        <v>52.7</v>
+        <v>976.45</v>
+      </c>
+      <c r="J25">
+        <v>1092.05</v>
       </c>
       <c r="K25" t="s">
         <v>15</v>
       </c>
       <c r="L25">
-        <v>48.8</v>
+        <v>911.3</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N25" t="s">
         <v>4</v>
@@ -1671,37 +1695,37 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <v>44491</v>
+        <v>44503</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>1243.3</v>
+        <v>467.25</v>
       </c>
       <c r="F26">
-        <v>1184.8599999999999</v>
+        <v>449.1</v>
       </c>
       <c r="G26">
-        <v>1112.71</v>
+        <v>434.55</v>
       </c>
       <c r="H26">
-        <v>1299.25</v>
+        <v>481.27</v>
       </c>
       <c r="I26">
-        <v>1328.27</v>
+        <v>483.37</v>
       </c>
       <c r="J26">
-        <v>1397.58</v>
+        <v>540.63</v>
       </c>
       <c r="K26" t="s">
         <v>15</v>
       </c>
       <c r="L26">
-        <v>1270.1500000000001</v>
+        <v>467.45</v>
       </c>
       <c r="M26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N26" t="s">
         <v>4</v>
@@ -1715,40 +1739,40 @@
         <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>44490</v>
+        <v>44503</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E27">
-        <v>14400.05</v>
+        <v>2376.5500000000002</v>
       </c>
       <c r="F27">
-        <v>13928.9</v>
+        <v>2227.59</v>
       </c>
       <c r="G27">
-        <v>13651.23</v>
+        <v>2195.98</v>
       </c>
       <c r="H27">
-        <v>14887.35</v>
+        <v>2447.7800000000002</v>
       </c>
       <c r="I27">
-        <v>15048.05</v>
+        <v>2447.85</v>
       </c>
       <c r="J27">
-        <v>15158.53</v>
+        <v>2581.4299999999998</v>
       </c>
       <c r="K27" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="L27">
-        <v>14644.95</v>
+        <v>2332.1</v>
       </c>
       <c r="M27">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N27" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -1759,40 +1783,40 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>44489</v>
+        <v>44503</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>14400</v>
+        <v>3960.1</v>
       </c>
       <c r="F28">
-        <v>13915.11</v>
+        <v>3811.12</v>
       </c>
       <c r="G28">
-        <v>13616.79</v>
+        <v>3778.9</v>
       </c>
       <c r="H28">
-        <v>14887.35</v>
+        <v>4078.9</v>
       </c>
       <c r="I28">
-        <v>15048</v>
+        <v>4094.88</v>
       </c>
       <c r="J28">
-        <v>15158.53</v>
+        <v>4611.7299999999996</v>
       </c>
       <c r="K28" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="L28">
-        <v>14453.9</v>
+        <v>4220.7</v>
       </c>
       <c r="M28">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N28" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -1803,34 +1827,34 @@
         <v>1</v>
       </c>
       <c r="C29" s="1">
-        <v>44489</v>
+        <v>44502</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E29">
-        <v>497.95</v>
+        <v>503</v>
       </c>
       <c r="F29">
-        <v>461.51</v>
+        <v>468.45</v>
       </c>
       <c r="G29">
-        <v>455.19</v>
+        <v>404.65</v>
       </c>
       <c r="H29">
-        <v>520.36</v>
+        <v>518.09</v>
       </c>
       <c r="I29">
-        <v>520.41999999999996</v>
+        <v>538.33000000000004</v>
       </c>
       <c r="J29">
-        <v>580.41999999999996</v>
+        <v>564.23</v>
       </c>
       <c r="K29" t="s">
         <v>6</v>
       </c>
       <c r="L29">
-        <v>428.55</v>
+        <v>407.5</v>
       </c>
       <c r="M29">
         <v>5</v>
@@ -1847,34 +1871,34 @@
         <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>44483</v>
+        <v>44498</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E30">
-        <v>8928</v>
+        <v>183.95</v>
       </c>
       <c r="F30">
-        <v>8199.61</v>
+        <v>172.67</v>
       </c>
       <c r="G30">
-        <v>8071.6</v>
+        <v>150.44</v>
       </c>
       <c r="H30">
-        <v>9329.76</v>
+        <v>189.47</v>
       </c>
       <c r="I30">
-        <v>9446.1</v>
+        <v>220.63</v>
       </c>
       <c r="K30" t="s">
         <v>15</v>
       </c>
       <c r="L30">
-        <v>9105.75</v>
+        <v>166.8</v>
       </c>
       <c r="M30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N30" t="s">
         <v>4</v>
@@ -1888,34 +1912,37 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <v>44483</v>
+        <v>44497</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E31">
-        <v>358</v>
+        <v>1947.1</v>
       </c>
       <c r="F31">
-        <v>327.27999999999997</v>
+        <v>1858.11</v>
       </c>
       <c r="G31">
-        <v>321.62</v>
+        <v>1845.66</v>
       </c>
       <c r="H31">
-        <v>374.11</v>
+        <v>2005.51</v>
       </c>
       <c r="I31">
-        <v>377.57</v>
+        <v>2022.07</v>
+      </c>
+      <c r="J31">
+        <v>2175.9699999999998</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L31">
-        <v>318.55</v>
+        <v>2149.5500000000002</v>
       </c>
       <c r="M31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N31" t="s">
         <v>4</v>
@@ -1929,40 +1956,37 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>44482</v>
+        <v>44491</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E32">
-        <v>1840.1</v>
+        <v>50.1</v>
       </c>
       <c r="F32">
-        <v>1728.38</v>
+        <v>46.38</v>
       </c>
       <c r="G32">
-        <v>1649.84</v>
+        <v>45.6</v>
       </c>
       <c r="H32">
-        <v>1922.9</v>
+        <v>52.35</v>
       </c>
       <c r="I32">
-        <v>1954.85</v>
-      </c>
-      <c r="J32">
-        <v>2179.75</v>
+        <v>52.7</v>
       </c>
       <c r="K32" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L32">
-        <v>1792.45</v>
+        <v>48.8</v>
       </c>
       <c r="M32">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -1973,34 +1997,34 @@
         <v>1</v>
       </c>
       <c r="C33" s="1">
-        <v>44481</v>
+        <v>44491</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E33">
-        <v>456.35</v>
+        <v>1243.3</v>
       </c>
       <c r="F33">
-        <v>431.76</v>
+        <v>1184.8599999999999</v>
       </c>
       <c r="G33">
-        <v>421.61</v>
+        <v>1112.71</v>
       </c>
       <c r="H33">
-        <v>476.89</v>
+        <v>1299.25</v>
       </c>
       <c r="I33">
-        <v>476.9</v>
+        <v>1328.27</v>
       </c>
       <c r="J33">
-        <v>531.9</v>
+        <v>1397.58</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
       </c>
       <c r="L33">
-        <v>464.65</v>
+        <v>1270.1500000000001</v>
       </c>
       <c r="M33">
         <v>2</v>
@@ -2017,40 +2041,40 @@
         <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>44481</v>
+        <v>44490</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E34">
-        <v>96.3</v>
+        <v>14400.05</v>
       </c>
       <c r="F34">
-        <v>91.74</v>
+        <v>13928.9</v>
       </c>
       <c r="G34">
-        <v>88.31</v>
+        <v>13651.23</v>
       </c>
       <c r="H34">
-        <v>100.63</v>
+        <v>14887.35</v>
       </c>
       <c r="I34">
-        <v>106.95</v>
+        <v>15048.05</v>
       </c>
       <c r="J34">
-        <v>122.7</v>
+        <v>15158.53</v>
       </c>
       <c r="K34" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="L34">
-        <v>102.55</v>
+        <v>14644.95</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="N34" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -2061,40 +2085,40 @@
         <v>1</v>
       </c>
       <c r="C35" s="1">
-        <v>44481</v>
+        <v>44489</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E35">
-        <v>2025</v>
+        <v>14400</v>
       </c>
       <c r="F35">
-        <v>1869.62</v>
+        <v>13915.11</v>
       </c>
       <c r="G35">
-        <v>1853.79</v>
+        <v>13616.79</v>
       </c>
       <c r="H35">
-        <v>2116.13</v>
+        <v>14887.35</v>
       </c>
       <c r="I35">
-        <v>2147.83</v>
+        <v>15048</v>
       </c>
       <c r="J35">
-        <v>2419.38</v>
+        <v>15158.53</v>
       </c>
       <c r="K35" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35">
+        <v>14453.9</v>
+      </c>
+      <c r="M35">
         <v>15</v>
       </c>
-      <c r="L35">
-        <v>1993.8</v>
-      </c>
-      <c r="M35">
-        <v>2</v>
-      </c>
       <c r="N35" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2105,37 +2129,37 @@
         <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>44480</v>
+        <v>44489</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E36">
-        <v>313.55</v>
+        <v>497.95</v>
       </c>
       <c r="F36">
-        <v>297.8</v>
+        <v>461.51</v>
       </c>
       <c r="G36">
-        <v>282.27</v>
+        <v>455.19</v>
       </c>
       <c r="H36">
-        <v>323.38</v>
+        <v>520.36</v>
       </c>
       <c r="I36">
-        <v>327.66000000000003</v>
+        <v>520.41999999999996</v>
       </c>
       <c r="J36">
-        <v>334.27</v>
+        <v>580.41999999999996</v>
       </c>
       <c r="K36" t="s">
         <v>6</v>
       </c>
       <c r="L36">
-        <v>269.75</v>
+        <v>428.55</v>
       </c>
       <c r="M36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N36" t="s">
         <v>6</v>
@@ -2149,37 +2173,34 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>44477</v>
+        <v>44483</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E37">
-        <v>789.25</v>
+        <v>8928</v>
       </c>
       <c r="F37">
-        <v>757.08</v>
+        <v>8199.61</v>
       </c>
       <c r="G37">
-        <v>751.14</v>
+        <v>8071.6</v>
       </c>
       <c r="H37">
-        <v>816.23</v>
+        <v>9329.76</v>
       </c>
       <c r="I37">
-        <v>824.77</v>
-      </c>
-      <c r="J37">
-        <v>834.78</v>
+        <v>9446.1</v>
       </c>
       <c r="K37" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L37">
-        <v>821</v>
+        <v>9105.75</v>
       </c>
       <c r="M37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N37" t="s">
         <v>4</v>
@@ -2193,40 +2214,37 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>44477</v>
+        <v>44483</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E38">
-        <v>656.4</v>
+        <v>358</v>
       </c>
       <c r="F38">
-        <v>653</v>
+        <v>327.27999999999997</v>
       </c>
       <c r="G38">
-        <v>632.46</v>
+        <v>321.62</v>
       </c>
       <c r="H38">
-        <v>685.94</v>
+        <v>374.11</v>
       </c>
       <c r="I38">
-        <v>708.65</v>
-      </c>
-      <c r="J38">
-        <v>792.4</v>
+        <v>377.57</v>
       </c>
       <c r="K38" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L38">
-        <v>515.79999999999995</v>
+        <v>318.55</v>
       </c>
       <c r="M38">
         <v>2</v>
       </c>
       <c r="N38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -2237,40 +2255,40 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>44477</v>
+        <v>44482</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E39">
-        <v>97.75</v>
+        <v>1840.1</v>
       </c>
       <c r="F39">
-        <v>90.97</v>
+        <v>1728.38</v>
       </c>
       <c r="G39">
-        <v>88.12</v>
+        <v>1649.84</v>
       </c>
       <c r="H39">
-        <v>102.15</v>
+        <v>1922.9</v>
       </c>
       <c r="I39">
-        <v>106.95</v>
+        <v>1954.85</v>
       </c>
       <c r="J39">
-        <v>122.7</v>
+        <v>2179.75</v>
       </c>
       <c r="K39" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="L39">
-        <v>97.45</v>
+        <v>1792.45</v>
       </c>
       <c r="M39">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N39" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -2281,37 +2299,37 @@
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>44477</v>
+        <v>44481</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E40">
-        <v>1965.1</v>
+        <v>456.35</v>
       </c>
       <c r="F40">
-        <v>1863.54</v>
+        <v>431.76</v>
       </c>
       <c r="G40">
-        <v>1850.86</v>
+        <v>421.61</v>
       </c>
       <c r="H40">
-        <v>2053.5300000000002</v>
+        <v>476.89</v>
       </c>
       <c r="I40">
-        <v>2073.9699999999998</v>
+        <v>476.9</v>
       </c>
       <c r="J40">
-        <v>2147.83</v>
+        <v>531.9</v>
       </c>
       <c r="K40" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L40">
-        <v>1946.05</v>
+        <v>464.65</v>
       </c>
       <c r="M40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N40" t="s">
         <v>4</v>
@@ -2325,37 +2343,37 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>44477</v>
+        <v>44481</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E41">
-        <v>211.55</v>
+        <v>96.3</v>
       </c>
       <c r="F41">
-        <v>199.66</v>
+        <v>91.74</v>
       </c>
       <c r="G41">
-        <v>195.14</v>
+        <v>88.31</v>
       </c>
       <c r="H41">
-        <v>221.07</v>
+        <v>100.63</v>
       </c>
       <c r="I41">
-        <v>222.5</v>
+        <v>106.95</v>
       </c>
       <c r="J41">
-        <v>231.5</v>
+        <v>122.7</v>
       </c>
       <c r="K41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L41">
-        <v>197.65</v>
+        <v>102.55</v>
       </c>
       <c r="M41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N41" t="s">
         <v>4</v>
@@ -2369,37 +2387,40 @@
         <v>1</v>
       </c>
       <c r="C42" s="1">
-        <v>44476</v>
+        <v>44481</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E42">
-        <v>2141.3000000000002</v>
+        <v>2025</v>
       </c>
       <c r="F42">
-        <v>1927.17</v>
+        <v>1869.62</v>
       </c>
       <c r="G42">
-        <v>1897.63</v>
+        <v>1853.79</v>
       </c>
       <c r="H42">
-        <v>2237.66</v>
+        <v>2116.13</v>
       </c>
       <c r="I42">
-        <v>2357.87</v>
+        <v>2147.83</v>
+      </c>
+      <c r="J42">
+        <v>2419.38</v>
       </c>
       <c r="K42" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="L42">
-        <v>1949.45</v>
+        <v>1993.8</v>
       </c>
       <c r="M42">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="N42" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -2410,37 +2431,40 @@
         <v>1</v>
       </c>
       <c r="C43" s="1">
-        <v>44476</v>
+        <v>44480</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E43">
-        <v>1304.5</v>
+        <v>313.55</v>
       </c>
       <c r="F43">
-        <v>1181.8499999999999</v>
+        <v>297.8</v>
       </c>
       <c r="G43">
-        <v>1177.8599999999999</v>
+        <v>282.27</v>
       </c>
       <c r="H43">
-        <v>1357.02</v>
+        <v>323.38</v>
       </c>
       <c r="I43">
-        <v>1363.2</v>
+        <v>327.66000000000003</v>
+      </c>
+      <c r="J43">
+        <v>334.27</v>
       </c>
       <c r="K43" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L43">
-        <v>1313.25</v>
+        <v>269.75</v>
       </c>
       <c r="M43">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N43" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -2451,37 +2475,40 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E44">
-        <v>1046</v>
+        <v>789.25</v>
       </c>
       <c r="F44">
-        <v>991.55</v>
+        <v>757.08</v>
       </c>
       <c r="G44">
-        <v>975.33</v>
+        <v>751.14</v>
       </c>
       <c r="H44">
-        <v>1093.07</v>
+        <v>816.23</v>
       </c>
       <c r="I44">
-        <v>1100.17</v>
+        <v>824.77</v>
+      </c>
+      <c r="J44">
+        <v>834.78</v>
       </c>
       <c r="K44" t="s">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>821</v>
+      </c>
+      <c r="M44">
         <v>6</v>
       </c>
-      <c r="L44">
-        <v>804.35</v>
-      </c>
-      <c r="M44">
-        <v>4</v>
-      </c>
       <c r="N44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -2492,37 +2519,37 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E45">
-        <v>310.7</v>
+        <v>656.4</v>
       </c>
       <c r="F45">
-        <v>295.52999999999997</v>
+        <v>653</v>
       </c>
       <c r="G45">
-        <v>280.48</v>
+        <v>632.46</v>
       </c>
       <c r="H45">
-        <v>323.38</v>
+        <v>685.94</v>
       </c>
       <c r="I45">
-        <v>324.68</v>
+        <v>708.65</v>
       </c>
       <c r="J45">
-        <v>334.27</v>
+        <v>792.4</v>
       </c>
       <c r="K45" t="s">
         <v>6</v>
       </c>
       <c r="L45">
-        <v>273.3</v>
+        <v>515.79999999999995</v>
       </c>
       <c r="M45">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N45" t="s">
         <v>6</v>
@@ -2536,40 +2563,40 @@
         <v>1</v>
       </c>
       <c r="C46" s="1">
-        <v>44475</v>
+        <v>44477</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E46">
-        <v>214.3</v>
+        <v>97.75</v>
       </c>
       <c r="F46">
-        <v>206.45</v>
+        <v>90.97</v>
       </c>
       <c r="G46">
-        <v>205.8</v>
+        <v>88.12</v>
       </c>
       <c r="H46">
-        <v>223.94</v>
+        <v>102.15</v>
       </c>
       <c r="I46">
-        <v>225.65</v>
+        <v>106.95</v>
       </c>
       <c r="J46">
-        <v>245.35</v>
+        <v>122.7</v>
       </c>
       <c r="K46" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="L46">
-        <v>214.4</v>
+        <v>97.45</v>
       </c>
       <c r="M46">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N46" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -2580,34 +2607,37 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <v>44474</v>
+        <v>44477</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E47">
-        <v>289</v>
+        <v>1965.1</v>
       </c>
       <c r="F47">
-        <v>276.52</v>
+        <v>1863.54</v>
       </c>
       <c r="G47">
-        <v>272.33</v>
+        <v>1850.86</v>
       </c>
       <c r="H47">
-        <v>302</v>
+        <v>2053.5300000000002</v>
       </c>
       <c r="I47">
-        <v>306.18</v>
+        <v>2073.9699999999998</v>
+      </c>
+      <c r="J47">
+        <v>2147.83</v>
       </c>
       <c r="K47" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L47">
-        <v>283.05</v>
+        <v>1946.05</v>
       </c>
       <c r="M47">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="N47" t="s">
         <v>4</v>
@@ -2621,39 +2651,335 @@
         <v>1</v>
       </c>
       <c r="C48" s="1">
-        <v>44470</v>
+        <v>44477</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E48">
-        <v>3396.6</v>
+        <v>211.55</v>
       </c>
       <c r="F48">
-        <v>3162.72</v>
+        <v>199.66</v>
       </c>
       <c r="G48">
-        <v>3027.58</v>
+        <v>195.14</v>
       </c>
       <c r="H48">
-        <v>3549.45</v>
+        <v>221.07</v>
       </c>
       <c r="I48">
-        <v>3557.23</v>
+        <v>222.5</v>
       </c>
       <c r="J48">
-        <v>3951.23</v>
+        <v>231.5</v>
       </c>
       <c r="K48" t="s">
         <v>15</v>
       </c>
       <c r="L48">
+        <v>197.65</v>
+      </c>
+      <c r="M48">
+        <v>5</v>
+      </c>
+      <c r="N48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49">
+        <v>2141.3000000000002</v>
+      </c>
+      <c r="F49">
+        <v>1927.17</v>
+      </c>
+      <c r="G49">
+        <v>1897.63</v>
+      </c>
+      <c r="H49">
+        <v>2237.66</v>
+      </c>
+      <c r="I49">
+        <v>2357.87</v>
+      </c>
+      <c r="K49" t="s">
+        <v>42</v>
+      </c>
+      <c r="L49">
+        <v>1949.45</v>
+      </c>
+      <c r="M49">
+        <v>15</v>
+      </c>
+      <c r="N49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>1304.5</v>
+      </c>
+      <c r="F50">
+        <v>1181.8499999999999</v>
+      </c>
+      <c r="G50">
+        <v>1177.8599999999999</v>
+      </c>
+      <c r="H50">
+        <v>1357.02</v>
+      </c>
+      <c r="I50">
+        <v>1363.2</v>
+      </c>
+      <c r="K50" t="s">
+        <v>15</v>
+      </c>
+      <c r="L50">
+        <v>1313.25</v>
+      </c>
+      <c r="M50">
+        <v>2</v>
+      </c>
+      <c r="N50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E51">
+        <v>1046</v>
+      </c>
+      <c r="F51">
+        <v>991.55</v>
+      </c>
+      <c r="G51">
+        <v>975.33</v>
+      </c>
+      <c r="H51">
+        <v>1093.07</v>
+      </c>
+      <c r="I51">
+        <v>1100.17</v>
+      </c>
+      <c r="K51" t="s">
+        <v>6</v>
+      </c>
+      <c r="L51">
+        <v>804.35</v>
+      </c>
+      <c r="M51">
+        <v>4</v>
+      </c>
+      <c r="N51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52">
+        <v>310.7</v>
+      </c>
+      <c r="F52">
+        <v>295.52999999999997</v>
+      </c>
+      <c r="G52">
+        <v>280.48</v>
+      </c>
+      <c r="H52">
+        <v>323.38</v>
+      </c>
+      <c r="I52">
+        <v>324.68</v>
+      </c>
+      <c r="J52">
+        <v>334.27</v>
+      </c>
+      <c r="K52" t="s">
+        <v>6</v>
+      </c>
+      <c r="L52">
+        <v>273.3</v>
+      </c>
+      <c r="M52">
+        <v>9</v>
+      </c>
+      <c r="N52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>44475</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>214.3</v>
+      </c>
+      <c r="F53">
+        <v>206.45</v>
+      </c>
+      <c r="G53">
+        <v>205.8</v>
+      </c>
+      <c r="H53">
+        <v>223.94</v>
+      </c>
+      <c r="I53">
+        <v>225.65</v>
+      </c>
+      <c r="J53">
+        <v>245.35</v>
+      </c>
+      <c r="K53" t="s">
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <v>214.4</v>
+      </c>
+      <c r="M53">
+        <v>9</v>
+      </c>
+      <c r="N53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>44474</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54">
+        <v>289</v>
+      </c>
+      <c r="F54">
+        <v>276.52</v>
+      </c>
+      <c r="G54">
+        <v>272.33</v>
+      </c>
+      <c r="H54">
+        <v>302</v>
+      </c>
+      <c r="I54">
+        <v>306.18</v>
+      </c>
+      <c r="K54" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54">
+        <v>283.05</v>
+      </c>
+      <c r="M54">
+        <v>13</v>
+      </c>
+      <c r="N54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>44470</v>
+      </c>
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55">
+        <v>3396.6</v>
+      </c>
+      <c r="F55">
+        <v>3162.72</v>
+      </c>
+      <c r="G55">
+        <v>3027.58</v>
+      </c>
+      <c r="H55">
+        <v>3549.45</v>
+      </c>
+      <c r="I55">
+        <v>3557.23</v>
+      </c>
+      <c r="J55">
+        <v>3951.23</v>
+      </c>
+      <c r="K55" t="s">
+        <v>15</v>
+      </c>
+      <c r="L55">
         <v>3392.4</v>
       </c>
-      <c r="M48">
+      <c r="M55">
         <v>7</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N55" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
report update feb 22
</commit_message>
<xml_diff>
--- a/default/data/Clean/NCASH.xlsx
+++ b/default/data/Clean/NCASH.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="69">
   <si>
     <t>Cash_N500</t>
   </si>
@@ -216,6 +216,21 @@
   </si>
   <si>
     <t>FLUOROCHEM.NS</t>
+  </si>
+  <si>
+    <t>UFLEX.NS</t>
+  </si>
+  <si>
+    <t>BALRAMCHIN.NS</t>
+  </si>
+  <si>
+    <t>GSFC.NS</t>
+  </si>
+  <si>
+    <t>FINEORG.NS</t>
+  </si>
+  <si>
+    <t>BHARATRAS.NS</t>
   </si>
 </sst>
 </file>
@@ -563,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,40 +645,40 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>44580</v>
+        <v>44617</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>1222.5</v>
+        <v>1981.95</v>
       </c>
       <c r="F2">
-        <v>1152.56</v>
+        <v>1978.68</v>
       </c>
       <c r="G2">
-        <v>1113.9000000000001</v>
+        <v>1958.01</v>
       </c>
       <c r="H2">
-        <v>1259.17</v>
+        <v>2034.08</v>
       </c>
       <c r="I2">
-        <v>1274.53</v>
+        <v>2041.41</v>
       </c>
       <c r="J2">
-        <v>1327.78</v>
+        <v>2090.85</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L2">
-        <v>1076.2</v>
+        <v>2027.45</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -674,37 +689,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>44575</v>
+        <v>44606</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="E3">
-        <v>499.65</v>
+        <v>553.25</v>
       </c>
       <c r="F3">
-        <v>468.25</v>
+        <v>534.80999999999995</v>
       </c>
       <c r="G3">
-        <v>464.03</v>
+        <v>520.91999999999996</v>
       </c>
       <c r="H3">
-        <v>514.64</v>
+        <v>569.85</v>
       </c>
       <c r="I3">
-        <v>515.6</v>
+        <v>584.75</v>
       </c>
       <c r="J3">
-        <v>529.22</v>
+        <v>651.35</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L3">
-        <v>488.3</v>
+        <v>519.9</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="s">
         <v>4</v>
@@ -718,37 +733,37 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>44573</v>
+        <v>44601</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>596.4</v>
+        <v>1324</v>
       </c>
       <c r="F4">
-        <v>568.29</v>
+        <v>1301.1600000000001</v>
       </c>
       <c r="G4">
-        <v>551.22</v>
+        <v>1293.48</v>
       </c>
       <c r="H4">
-        <v>614.29</v>
+        <v>1363.72</v>
       </c>
       <c r="I4">
-        <v>669</v>
+        <v>1423.83</v>
       </c>
       <c r="J4">
-        <v>780.4</v>
+        <v>1570.18</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
       <c r="L4">
-        <v>599.45000000000005</v>
+        <v>1216.9000000000001</v>
       </c>
       <c r="M4">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N4" t="s">
         <v>6</v>
@@ -762,40 +777,40 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>44571</v>
+        <v>44599</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E5">
-        <v>31.8</v>
+        <v>452.75</v>
       </c>
       <c r="F5">
-        <v>29.37</v>
+        <v>430.28</v>
       </c>
       <c r="G5">
-        <v>28.98</v>
+        <v>377.77</v>
       </c>
       <c r="H5">
-        <v>32.75</v>
+        <v>466.33</v>
       </c>
       <c r="I5">
-        <v>32.799999999999997</v>
+        <v>468.63</v>
       </c>
       <c r="J5">
-        <v>33.520000000000003</v>
+        <v>490.85</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L5">
-        <v>30.65</v>
+        <v>391.9</v>
       </c>
       <c r="M5">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -806,37 +821,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>44571</v>
+        <v>44599</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>382.05</v>
+        <v>2142</v>
       </c>
       <c r="F6">
-        <v>367</v>
+        <v>2069.15</v>
       </c>
       <c r="G6">
-        <v>356.22</v>
+        <v>2052.2199999999998</v>
       </c>
       <c r="H6">
-        <v>391.12</v>
+        <v>2206.2600000000002</v>
       </c>
       <c r="I6">
-        <v>393.51</v>
-      </c>
-      <c r="J6">
-        <v>403.35</v>
+        <v>2250.3000000000002</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <v>434.7</v>
+        <v>2176.9499999999998</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N6" t="s">
         <v>4</v>
@@ -850,40 +862,40 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>44568</v>
+        <v>44599</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="E7">
-        <v>158.69999999999999</v>
+        <v>133.6</v>
       </c>
       <c r="F7">
-        <v>147.59</v>
+        <v>128.38</v>
       </c>
       <c r="G7">
-        <v>147.49</v>
+        <v>124.6</v>
       </c>
       <c r="H7">
-        <v>163.46</v>
+        <v>137.61000000000001</v>
       </c>
       <c r="I7">
-        <v>166.75</v>
+        <v>138.07</v>
       </c>
       <c r="J7">
-        <v>184.75</v>
+        <v>142.80000000000001</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L7">
-        <v>157.75</v>
+        <v>121.6</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -894,40 +906,40 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>44568</v>
+        <v>44596</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E8">
-        <v>200.65</v>
+        <v>4092</v>
       </c>
       <c r="F8">
-        <v>190.7</v>
+        <v>3776.95</v>
       </c>
       <c r="G8">
-        <v>183.28</v>
+        <v>3746.76</v>
       </c>
       <c r="H8">
-        <v>206.67</v>
+        <v>4214.76</v>
       </c>
       <c r="I8">
-        <v>214.8</v>
+        <v>4242.17</v>
       </c>
       <c r="J8">
-        <v>223.1</v>
+        <v>4730.0200000000004</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L8">
-        <v>201.05</v>
+        <v>3947.4</v>
       </c>
       <c r="M8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -938,40 +950,40 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>44566</v>
+        <v>44595</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E9">
-        <v>1903.9</v>
+        <v>13206</v>
       </c>
       <c r="F9">
-        <v>1755.34</v>
+        <v>12389.2</v>
       </c>
       <c r="G9">
-        <v>1642.64</v>
+        <v>12025.37</v>
       </c>
       <c r="H9">
-        <v>1961.02</v>
+        <v>13579.15</v>
       </c>
       <c r="I9">
-        <v>1969.95</v>
+        <v>13602.18</v>
       </c>
       <c r="J9">
-        <v>2061.4699999999998</v>
+        <v>13936.05</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L9">
-        <v>1977.45</v>
+        <v>12185.55</v>
       </c>
       <c r="M9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -982,40 +994,40 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>44539</v>
+        <v>44580</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E10">
-        <v>2228.5</v>
+        <v>1222.5</v>
       </c>
       <c r="F10">
-        <v>2108.85</v>
+        <v>1152.56</v>
       </c>
       <c r="G10">
-        <v>1997.53</v>
+        <v>1113.9000000000001</v>
       </c>
       <c r="H10">
-        <v>2295.36</v>
+        <v>1259.17</v>
       </c>
       <c r="I10">
-        <v>2360.58</v>
+        <v>1274.53</v>
       </c>
       <c r="J10">
-        <v>2638.53</v>
+        <v>1327.78</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L10">
-        <v>2226.6</v>
+        <v>1048.5999999999999</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1026,37 +1038,37 @@
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>44533</v>
+        <v>44575</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>364.15</v>
+        <v>499.65</v>
       </c>
       <c r="F11">
-        <v>337.79</v>
+        <v>468.25</v>
       </c>
       <c r="G11">
-        <v>318.74</v>
+        <v>464.03</v>
       </c>
       <c r="H11">
-        <v>375.07</v>
+        <v>514.64</v>
       </c>
       <c r="I11">
-        <v>385.52</v>
+        <v>515.6</v>
       </c>
       <c r="J11">
-        <v>403.45</v>
+        <v>529.22</v>
       </c>
       <c r="K11" t="s">
         <v>3</v>
       </c>
       <c r="L11">
-        <v>424</v>
+        <v>469.95</v>
       </c>
       <c r="M11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N11" t="s">
         <v>4</v>
@@ -1070,37 +1082,37 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>44533</v>
+        <v>44573</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="E12">
-        <v>154.94999999999999</v>
+        <v>596.4</v>
       </c>
       <c r="F12">
-        <v>151.22</v>
+        <v>568.29</v>
       </c>
       <c r="G12">
-        <v>147.36000000000001</v>
+        <v>551.22</v>
       </c>
       <c r="H12">
-        <v>159.6</v>
+        <v>614.29</v>
       </c>
       <c r="I12">
-        <v>160.97999999999999</v>
+        <v>669</v>
       </c>
       <c r="J12">
-        <v>167.95</v>
+        <v>780.4</v>
       </c>
       <c r="K12" t="s">
         <v>6</v>
       </c>
       <c r="L12">
-        <v>145.9</v>
+        <v>676.55</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="N12" t="s">
         <v>6</v>
@@ -1114,40 +1126,40 @@
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>44531</v>
+        <v>44571</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="E13">
-        <v>5080.25</v>
+        <v>31.8</v>
       </c>
       <c r="F13">
-        <v>4957.96</v>
+        <v>29.37</v>
       </c>
       <c r="G13">
-        <v>4845.8599999999997</v>
+        <v>28.98</v>
       </c>
       <c r="H13">
-        <v>5220.53</v>
+        <v>32.75</v>
       </c>
       <c r="I13">
-        <v>5232.66</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="J13">
-        <v>5311.9</v>
+        <v>33.520000000000003</v>
       </c>
       <c r="K13" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="L13">
-        <v>5060.1000000000004</v>
+        <v>30.65</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="N13" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1158,37 +1170,37 @@
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>44526</v>
+        <v>44571</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E14">
-        <v>1810.1</v>
+        <v>382.05</v>
       </c>
       <c r="F14">
-        <v>1745.93</v>
+        <v>367</v>
       </c>
       <c r="G14">
-        <v>1715.01</v>
+        <v>356.22</v>
       </c>
       <c r="H14">
-        <v>1864.4</v>
+        <v>391.12</v>
       </c>
       <c r="I14">
-        <v>1887.2</v>
+        <v>393.51</v>
       </c>
       <c r="J14">
-        <v>2088.1999999999998</v>
+        <v>403.35</v>
       </c>
       <c r="K14" t="s">
         <v>3</v>
       </c>
       <c r="L14">
-        <v>1974.55</v>
+        <v>434.7</v>
       </c>
       <c r="M14">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N14" t="s">
         <v>4</v>
@@ -1202,37 +1214,37 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>44522</v>
+        <v>44568</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>142.9</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="F15">
-        <v>133.26</v>
+        <v>147.59</v>
       </c>
       <c r="G15">
-        <v>127.28</v>
+        <v>147.49</v>
       </c>
       <c r="H15">
-        <v>147.19</v>
+        <v>163.46</v>
       </c>
       <c r="I15">
-        <v>149.35</v>
+        <v>166.75</v>
       </c>
       <c r="J15">
-        <v>156.41999999999999</v>
+        <v>184.75</v>
       </c>
       <c r="K15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L15">
-        <v>149.30000000000001</v>
+        <v>157.75</v>
       </c>
       <c r="M15">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N15" t="s">
         <v>4</v>
@@ -1246,40 +1258,40 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>44517</v>
+        <v>44568</v>
       </c>
       <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>200.65</v>
+      </c>
+      <c r="F16">
+        <v>190.7</v>
+      </c>
+      <c r="G16">
+        <v>183.28</v>
+      </c>
+      <c r="H16">
+        <v>206.67</v>
+      </c>
+      <c r="I16">
+        <v>214.8</v>
+      </c>
+      <c r="J16">
+        <v>223.1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>201.05</v>
+      </c>
+      <c r="M16">
         <v>10</v>
       </c>
-      <c r="E16">
-        <v>230.3</v>
-      </c>
-      <c r="F16">
-        <v>218.03</v>
-      </c>
-      <c r="G16">
-        <v>214.41</v>
-      </c>
-      <c r="H16">
-        <v>237.21</v>
-      </c>
-      <c r="I16">
-        <v>241.3</v>
-      </c>
-      <c r="J16">
-        <v>258</v>
-      </c>
-      <c r="K16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16">
-        <v>213.5</v>
-      </c>
-      <c r="M16">
-        <v>4</v>
-      </c>
       <c r="N16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1290,40 +1302,40 @@
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>44516</v>
+        <v>44566</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E17">
-        <v>504</v>
+        <v>1903.9</v>
       </c>
       <c r="F17">
-        <v>485.12</v>
+        <v>1755.34</v>
       </c>
       <c r="G17">
-        <v>474.56</v>
+        <v>1642.64</v>
       </c>
       <c r="H17">
-        <v>519.12</v>
+        <v>1961.02</v>
       </c>
       <c r="I17">
-        <v>564.98</v>
+        <v>1969.95</v>
       </c>
       <c r="J17">
-        <v>657.23</v>
+        <v>2061.4699999999998</v>
       </c>
       <c r="K17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L17">
-        <v>425.5</v>
+        <v>1977.45</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1334,40 +1346,40 @@
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>44516</v>
+        <v>44539</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>2288.75</v>
+        <v>2228.5</v>
       </c>
       <c r="F18">
-        <v>2194.21</v>
+        <v>2108.85</v>
       </c>
       <c r="G18">
-        <v>2184.1799999999998</v>
+        <v>1997.53</v>
       </c>
       <c r="H18">
-        <v>2357.41</v>
+        <v>2295.36</v>
       </c>
       <c r="I18">
-        <v>2392.4499999999998</v>
+        <v>2360.58</v>
       </c>
       <c r="J18">
-        <v>2609.85</v>
+        <v>2638.53</v>
       </c>
       <c r="K18" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L18">
-        <v>1911.7</v>
+        <v>2226.6</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1378,40 +1390,40 @@
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>44515</v>
+        <v>44533</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>367.8</v>
+        <v>364.15</v>
       </c>
       <c r="F19">
-        <v>356.44</v>
+        <v>337.79</v>
       </c>
       <c r="G19">
-        <v>341.13</v>
+        <v>318.74</v>
       </c>
       <c r="H19">
-        <v>378.83</v>
+        <v>375.07</v>
       </c>
       <c r="I19">
-        <v>387.22</v>
+        <v>385.52</v>
       </c>
       <c r="J19">
-        <v>433.87</v>
+        <v>403.45</v>
       </c>
       <c r="K19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L19">
-        <v>374.15</v>
+        <v>424</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1422,40 +1434,40 @@
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>44515</v>
+        <v>44533</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>926.25</v>
+        <v>154.94999999999999</v>
       </c>
       <c r="F20">
-        <v>869.94</v>
+        <v>151.22</v>
       </c>
       <c r="G20">
-        <v>866.86</v>
+        <v>147.36000000000001</v>
       </c>
       <c r="H20">
-        <v>954.04</v>
+        <v>159.6</v>
       </c>
       <c r="I20">
-        <v>959.1</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="J20">
-        <v>1056.0999999999999</v>
+        <v>167.95</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L20">
-        <v>918.2</v>
+        <v>145.9</v>
       </c>
       <c r="M20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1466,37 +1478,37 @@
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>44512</v>
+        <v>44531</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E21">
-        <v>922.15</v>
+        <v>5080.25</v>
       </c>
       <c r="F21">
-        <v>866.97</v>
+        <v>4957.96</v>
       </c>
       <c r="G21">
-        <v>846.17</v>
+        <v>4845.8599999999997</v>
       </c>
       <c r="H21">
-        <v>949.81</v>
+        <v>5220.53</v>
       </c>
       <c r="I21">
-        <v>959.97</v>
+        <v>5232.66</v>
       </c>
       <c r="J21">
-        <v>1104.8699999999999</v>
+        <v>5311.9</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="L21">
-        <v>925.35</v>
+        <v>5060.1000000000004</v>
       </c>
       <c r="M21">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N21" t="s">
         <v>4</v>
@@ -1510,40 +1522,40 @@
         <v>1</v>
       </c>
       <c r="C22" s="1">
-        <v>44512</v>
+        <v>44526</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>2252.3000000000002</v>
+        <v>1810.1</v>
       </c>
       <c r="F22">
-        <v>2189.8000000000002</v>
+        <v>1745.93</v>
       </c>
       <c r="G22">
-        <v>2179.61</v>
+        <v>1715.01</v>
       </c>
       <c r="H22">
-        <v>2319.87</v>
+        <v>1864.4</v>
       </c>
       <c r="I22">
-        <v>2392.4499999999998</v>
+        <v>1887.2</v>
       </c>
       <c r="J22">
-        <v>2609.85</v>
+        <v>2088.1999999999998</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L22">
-        <v>2042.05</v>
+        <v>1974.55</v>
       </c>
       <c r="M22">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1554,37 +1566,37 @@
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>44510</v>
+        <v>44522</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E23">
-        <v>4169.55</v>
+        <v>142.9</v>
       </c>
       <c r="F23">
-        <v>4107.1499999999996</v>
+        <v>133.26</v>
       </c>
       <c r="G23">
-        <v>3788.59</v>
+        <v>127.28</v>
       </c>
       <c r="H23">
-        <v>4294.6400000000003</v>
+        <v>147.19</v>
       </c>
       <c r="I23">
-        <v>4574.22</v>
+        <v>149.35</v>
       </c>
       <c r="J23">
-        <v>4830.2700000000004</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="K23" t="s">
         <v>3</v>
       </c>
       <c r="L23">
-        <v>3861.95</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="M23">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N23" t="s">
         <v>4</v>
@@ -1598,40 +1610,40 @@
         <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>44509</v>
+        <v>44517</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="E24">
-        <v>2006.35</v>
+        <v>230.3</v>
       </c>
       <c r="F24">
-        <v>1940.16</v>
+        <v>218.03</v>
       </c>
       <c r="G24">
-        <v>1849.85</v>
+        <v>214.41</v>
       </c>
       <c r="H24">
-        <v>2066.54</v>
+        <v>237.21</v>
       </c>
       <c r="I24">
-        <v>2111.6</v>
+        <v>241.3</v>
       </c>
       <c r="J24">
-        <v>2406.8000000000002</v>
+        <v>258</v>
       </c>
       <c r="K24" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L24">
-        <v>1966.85</v>
+        <v>213.5</v>
       </c>
       <c r="M24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1642,37 +1654,37 @@
         <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>44504</v>
+        <v>44516</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E25">
-        <v>1438</v>
+        <v>504</v>
       </c>
       <c r="F25">
-        <v>1348.05</v>
+        <v>485.12</v>
       </c>
       <c r="G25">
-        <v>1246.52</v>
+        <v>474.56</v>
       </c>
       <c r="H25">
-        <v>1481.14</v>
+        <v>519.12</v>
       </c>
       <c r="I25">
-        <v>1500.53</v>
+        <v>564.98</v>
       </c>
       <c r="J25">
-        <v>1557.03</v>
+        <v>657.23</v>
       </c>
       <c r="K25" t="s">
         <v>6</v>
       </c>
       <c r="L25">
-        <v>1292.45</v>
+        <v>425.5</v>
       </c>
       <c r="M25">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N25" t="s">
         <v>6</v>
@@ -1686,40 +1698,40 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <v>44503</v>
+        <v>44516</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>940</v>
+        <v>2288.75</v>
       </c>
       <c r="F26">
-        <v>889.59</v>
+        <v>2194.21</v>
       </c>
       <c r="G26">
-        <v>877.45</v>
+        <v>2184.1799999999998</v>
       </c>
       <c r="H26">
-        <v>968.2</v>
+        <v>2357.41</v>
       </c>
       <c r="I26">
-        <v>976.45</v>
+        <v>2392.4499999999998</v>
       </c>
       <c r="J26">
-        <v>1092.05</v>
+        <v>2609.85</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L26">
-        <v>911.3</v>
+        <v>1911.7</v>
       </c>
       <c r="M26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -1730,40 +1742,40 @@
         <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>44503</v>
+        <v>44515</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E27">
-        <v>467.25</v>
+        <v>367.8</v>
       </c>
       <c r="F27">
-        <v>449.1</v>
+        <v>356.44</v>
       </c>
       <c r="G27">
-        <v>434.55</v>
+        <v>341.13</v>
       </c>
       <c r="H27">
-        <v>481.27</v>
+        <v>378.83</v>
       </c>
       <c r="I27">
-        <v>483.37</v>
+        <v>387.22</v>
       </c>
       <c r="J27">
-        <v>540.63</v>
+        <v>433.87</v>
       </c>
       <c r="K27" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L27">
-        <v>467.45</v>
+        <v>374.15</v>
       </c>
       <c r="M27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -1774,37 +1786,37 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>44503</v>
+        <v>44515</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <v>2376.5500000000002</v>
+        <v>926.25</v>
       </c>
       <c r="F28">
-        <v>2227.59</v>
+        <v>869.94</v>
       </c>
       <c r="G28">
-        <v>2195.98</v>
+        <v>866.86</v>
       </c>
       <c r="H28">
-        <v>2447.7800000000002</v>
+        <v>954.04</v>
       </c>
       <c r="I28">
-        <v>2447.85</v>
+        <v>959.1</v>
       </c>
       <c r="J28">
-        <v>2581.4299999999998</v>
+        <v>1056.0999999999999</v>
       </c>
       <c r="K28" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L28">
-        <v>2332.1</v>
+        <v>918.2</v>
       </c>
       <c r="M28">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N28" t="s">
         <v>4</v>
@@ -1818,37 +1830,37 @@
         <v>1</v>
       </c>
       <c r="C29" s="1">
-        <v>44503</v>
+        <v>44512</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>3960.1</v>
+        <v>922.15</v>
       </c>
       <c r="F29">
-        <v>3811.12</v>
+        <v>866.97</v>
       </c>
       <c r="G29">
-        <v>3778.9</v>
+        <v>846.17</v>
       </c>
       <c r="H29">
-        <v>4078.9</v>
+        <v>949.81</v>
       </c>
       <c r="I29">
-        <v>4094.88</v>
+        <v>959.97</v>
       </c>
       <c r="J29">
-        <v>4611.7299999999996</v>
+        <v>1104.8699999999999</v>
       </c>
       <c r="K29" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="L29">
-        <v>4220.7</v>
+        <v>925.35</v>
       </c>
       <c r="M29">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N29" t="s">
         <v>4</v>
@@ -1862,37 +1874,37 @@
         <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>44502</v>
+        <v>44512</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E30">
-        <v>503</v>
+        <v>2252.3000000000002</v>
       </c>
       <c r="F30">
-        <v>468.45</v>
+        <v>2189.8000000000002</v>
       </c>
       <c r="G30">
-        <v>404.65</v>
+        <v>2179.61</v>
       </c>
       <c r="H30">
-        <v>518.09</v>
+        <v>2319.87</v>
       </c>
       <c r="I30">
-        <v>538.33000000000004</v>
+        <v>2392.4499999999998</v>
       </c>
       <c r="J30">
-        <v>564.23</v>
+        <v>2609.85</v>
       </c>
       <c r="K30" t="s">
         <v>6</v>
       </c>
       <c r="L30">
-        <v>407.5</v>
+        <v>2042.05</v>
       </c>
       <c r="M30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N30" t="s">
         <v>6</v>
@@ -1906,34 +1918,37 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <v>44498</v>
+        <v>44510</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E31">
-        <v>183.95</v>
+        <v>4169.55</v>
       </c>
       <c r="F31">
-        <v>172.67</v>
+        <v>4107.1499999999996</v>
       </c>
       <c r="G31">
-        <v>150.44</v>
+        <v>3788.59</v>
       </c>
       <c r="H31">
-        <v>189.47</v>
+        <v>4294.6400000000003</v>
       </c>
       <c r="I31">
-        <v>220.63</v>
+        <v>4574.22</v>
+      </c>
+      <c r="J31">
+        <v>4830.2700000000004</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L31">
-        <v>166.8</v>
+        <v>3861.95</v>
       </c>
       <c r="M31">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N31" t="s">
         <v>4</v>
@@ -1947,37 +1962,37 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>44497</v>
+        <v>44509</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E32">
-        <v>1947.1</v>
+        <v>2006.35</v>
       </c>
       <c r="F32">
-        <v>1858.11</v>
+        <v>1940.16</v>
       </c>
       <c r="G32">
-        <v>1845.66</v>
+        <v>1849.85</v>
       </c>
       <c r="H32">
-        <v>2005.51</v>
+        <v>2066.54</v>
       </c>
       <c r="I32">
-        <v>2022.07</v>
+        <v>2111.6</v>
       </c>
       <c r="J32">
-        <v>2175.9699999999998</v>
+        <v>2406.8000000000002</v>
       </c>
       <c r="K32" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L32">
-        <v>2149.5500000000002</v>
+        <v>1966.85</v>
       </c>
       <c r="M32">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N32" t="s">
         <v>4</v>
@@ -1991,37 +2006,40 @@
         <v>1</v>
       </c>
       <c r="C33" s="1">
-        <v>44491</v>
+        <v>44504</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E33">
-        <v>50.1</v>
+        <v>1438</v>
       </c>
       <c r="F33">
-        <v>46.38</v>
+        <v>1348.05</v>
       </c>
       <c r="G33">
-        <v>45.6</v>
+        <v>1246.52</v>
       </c>
       <c r="H33">
-        <v>52.35</v>
+        <v>1481.14</v>
       </c>
       <c r="I33">
-        <v>52.7</v>
+        <v>1500.53</v>
+      </c>
+      <c r="J33">
+        <v>1557.03</v>
       </c>
       <c r="K33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L33">
-        <v>48.8</v>
+        <v>1292.45</v>
       </c>
       <c r="M33">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N33" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -2032,37 +2050,37 @@
         <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>44491</v>
+        <v>44503</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E34">
-        <v>1243.3</v>
+        <v>940</v>
       </c>
       <c r="F34">
-        <v>1184.8599999999999</v>
+        <v>889.59</v>
       </c>
       <c r="G34">
-        <v>1112.71</v>
+        <v>877.45</v>
       </c>
       <c r="H34">
-        <v>1299.25</v>
+        <v>968.2</v>
       </c>
       <c r="I34">
-        <v>1328.27</v>
+        <v>976.45</v>
       </c>
       <c r="J34">
-        <v>1397.58</v>
+        <v>1092.05</v>
       </c>
       <c r="K34" t="s">
         <v>15</v>
       </c>
       <c r="L34">
-        <v>1270.1500000000001</v>
+        <v>911.3</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N34" t="s">
         <v>4</v>
@@ -2076,40 +2094,40 @@
         <v>1</v>
       </c>
       <c r="C35" s="1">
-        <v>44490</v>
+        <v>44503</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="E35">
-        <v>14400.05</v>
+        <v>467.25</v>
       </c>
       <c r="F35">
-        <v>13928.9</v>
+        <v>449.1</v>
       </c>
       <c r="G35">
-        <v>13651.23</v>
+        <v>434.55</v>
       </c>
       <c r="H35">
-        <v>14887.35</v>
+        <v>481.27</v>
       </c>
       <c r="I35">
-        <v>15048.05</v>
+        <v>483.37</v>
       </c>
       <c r="J35">
-        <v>15158.53</v>
+        <v>540.63</v>
       </c>
       <c r="K35" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="L35">
-        <v>14644.95</v>
+        <v>467.45</v>
       </c>
       <c r="M35">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="N35" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2120,40 +2138,40 @@
         <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>44489</v>
+        <v>44503</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E36">
-        <v>14400</v>
+        <v>2376.5500000000002</v>
       </c>
       <c r="F36">
-        <v>13915.11</v>
+        <v>2227.59</v>
       </c>
       <c r="G36">
-        <v>13616.79</v>
+        <v>2195.98</v>
       </c>
       <c r="H36">
-        <v>14887.35</v>
+        <v>2447.7800000000002</v>
       </c>
       <c r="I36">
-        <v>15048</v>
+        <v>2447.85</v>
       </c>
       <c r="J36">
-        <v>15158.53</v>
+        <v>2581.4299999999998</v>
       </c>
       <c r="K36" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="L36">
-        <v>14453.9</v>
+        <v>2332.1</v>
       </c>
       <c r="M36">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N36" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -2164,40 +2182,40 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>44489</v>
+        <v>44503</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E37">
-        <v>497.95</v>
+        <v>3960.1</v>
       </c>
       <c r="F37">
-        <v>461.51</v>
+        <v>3811.12</v>
       </c>
       <c r="G37">
-        <v>455.19</v>
+        <v>3778.9</v>
       </c>
       <c r="H37">
-        <v>520.36</v>
+        <v>4078.9</v>
       </c>
       <c r="I37">
-        <v>520.41999999999996</v>
+        <v>4094.88</v>
       </c>
       <c r="J37">
-        <v>580.41999999999996</v>
+        <v>4611.7299999999996</v>
       </c>
       <c r="K37" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L37">
-        <v>428.55</v>
+        <v>4220.7</v>
       </c>
       <c r="M37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -2208,37 +2226,40 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>44483</v>
+        <v>44502</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E38">
-        <v>8928</v>
+        <v>503</v>
       </c>
       <c r="F38">
-        <v>8199.61</v>
+        <v>468.45</v>
       </c>
       <c r="G38">
-        <v>8071.6</v>
+        <v>404.65</v>
       </c>
       <c r="H38">
-        <v>9329.76</v>
+        <v>518.09</v>
       </c>
       <c r="I38">
-        <v>9446.1</v>
+        <v>538.33000000000004</v>
+      </c>
+      <c r="J38">
+        <v>564.23</v>
       </c>
       <c r="K38" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L38">
-        <v>9105.75</v>
+        <v>407.5</v>
       </c>
       <c r="M38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -2249,34 +2270,34 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>44483</v>
+        <v>44498</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E39">
-        <v>358</v>
+        <v>183.95</v>
       </c>
       <c r="F39">
-        <v>327.27999999999997</v>
+        <v>172.67</v>
       </c>
       <c r="G39">
-        <v>321.62</v>
+        <v>150.44</v>
       </c>
       <c r="H39">
-        <v>374.11</v>
+        <v>189.47</v>
       </c>
       <c r="I39">
-        <v>377.57</v>
+        <v>220.63</v>
       </c>
       <c r="K39" t="s">
         <v>15</v>
       </c>
       <c r="L39">
-        <v>318.55</v>
+        <v>166.8</v>
       </c>
       <c r="M39">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N39" t="s">
         <v>4</v>
@@ -2290,40 +2311,40 @@
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>44482</v>
+        <v>44497</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E40">
-        <v>1840.1</v>
+        <v>1947.1</v>
       </c>
       <c r="F40">
-        <v>1728.38</v>
+        <v>1858.11</v>
       </c>
       <c r="G40">
-        <v>1649.84</v>
+        <v>1845.66</v>
       </c>
       <c r="H40">
-        <v>1922.9</v>
+        <v>2005.51</v>
       </c>
       <c r="I40">
-        <v>1954.85</v>
+        <v>2022.07</v>
       </c>
       <c r="J40">
-        <v>2179.75</v>
+        <v>2175.9699999999998</v>
       </c>
       <c r="K40" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L40">
-        <v>1792.45</v>
+        <v>2149.5500000000002</v>
       </c>
       <c r="M40">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -2334,37 +2355,34 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>44481</v>
+        <v>44491</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E41">
-        <v>456.35</v>
+        <v>50.1</v>
       </c>
       <c r="F41">
-        <v>431.76</v>
+        <v>46.38</v>
       </c>
       <c r="G41">
-        <v>421.61</v>
+        <v>45.6</v>
       </c>
       <c r="H41">
-        <v>476.89</v>
+        <v>52.35</v>
       </c>
       <c r="I41">
-        <v>476.9</v>
-      </c>
-      <c r="J41">
-        <v>531.9</v>
+        <v>52.7</v>
       </c>
       <c r="K41" t="s">
         <v>15</v>
       </c>
       <c r="L41">
-        <v>464.65</v>
+        <v>48.8</v>
       </c>
       <c r="M41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N41" t="s">
         <v>4</v>
@@ -2378,34 +2396,34 @@
         <v>1</v>
       </c>
       <c r="C42" s="1">
-        <v>44481</v>
+        <v>44491</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E42">
-        <v>96.3</v>
+        <v>1243.3</v>
       </c>
       <c r="F42">
-        <v>91.74</v>
+        <v>1184.8599999999999</v>
       </c>
       <c r="G42">
-        <v>88.31</v>
+        <v>1112.71</v>
       </c>
       <c r="H42">
-        <v>100.63</v>
+        <v>1299.25</v>
       </c>
       <c r="I42">
-        <v>106.95</v>
+        <v>1328.27</v>
       </c>
       <c r="J42">
-        <v>122.7</v>
+        <v>1397.58</v>
       </c>
       <c r="K42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L42">
-        <v>102.55</v>
+        <v>1270.1500000000001</v>
       </c>
       <c r="M42">
         <v>2</v>
@@ -2422,40 +2440,40 @@
         <v>1</v>
       </c>
       <c r="C43" s="1">
-        <v>44481</v>
+        <v>44490</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E43">
-        <v>2025</v>
+        <v>14400.05</v>
       </c>
       <c r="F43">
-        <v>1869.62</v>
+        <v>13928.9</v>
       </c>
       <c r="G43">
-        <v>1853.79</v>
+        <v>13651.23</v>
       </c>
       <c r="H43">
-        <v>2116.13</v>
+        <v>14887.35</v>
       </c>
       <c r="I43">
-        <v>2147.83</v>
+        <v>15048.05</v>
       </c>
       <c r="J43">
-        <v>2419.38</v>
+        <v>15158.53</v>
       </c>
       <c r="K43" t="s">
+        <v>41</v>
+      </c>
+      <c r="L43">
+        <v>14644.95</v>
+      </c>
+      <c r="M43">
         <v>15</v>
       </c>
-      <c r="L43">
-        <v>1993.8</v>
-      </c>
-      <c r="M43">
-        <v>2</v>
-      </c>
       <c r="N43" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -2466,40 +2484,40 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>44480</v>
+        <v>44489</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E44">
-        <v>313.55</v>
+        <v>14400</v>
       </c>
       <c r="F44">
-        <v>297.8</v>
+        <v>13915.11</v>
       </c>
       <c r="G44">
-        <v>282.27</v>
+        <v>13616.79</v>
       </c>
       <c r="H44">
-        <v>323.38</v>
+        <v>14887.35</v>
       </c>
       <c r="I44">
-        <v>327.66000000000003</v>
+        <v>15048</v>
       </c>
       <c r="J44">
-        <v>334.27</v>
+        <v>15158.53</v>
       </c>
       <c r="K44" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L44">
-        <v>269.75</v>
+        <v>14453.9</v>
       </c>
       <c r="M44">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="N44" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -2510,40 +2528,40 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <v>44477</v>
+        <v>44489</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E45">
-        <v>789.25</v>
+        <v>497.95</v>
       </c>
       <c r="F45">
-        <v>757.08</v>
+        <v>461.51</v>
       </c>
       <c r="G45">
-        <v>751.14</v>
+        <v>455.19</v>
       </c>
       <c r="H45">
-        <v>816.23</v>
+        <v>520.36</v>
       </c>
       <c r="I45">
-        <v>824.77</v>
+        <v>520.41999999999996</v>
       </c>
       <c r="J45">
-        <v>834.78</v>
+        <v>580.41999999999996</v>
       </c>
       <c r="K45" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L45">
-        <v>821</v>
+        <v>428.55</v>
       </c>
       <c r="M45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -2554,40 +2572,37 @@
         <v>1</v>
       </c>
       <c r="C46" s="1">
-        <v>44477</v>
+        <v>44483</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E46">
-        <v>656.4</v>
+        <v>8928</v>
       </c>
       <c r="F46">
-        <v>653</v>
+        <v>8199.61</v>
       </c>
       <c r="G46">
-        <v>632.46</v>
+        <v>8071.6</v>
       </c>
       <c r="H46">
-        <v>685.94</v>
+        <v>9329.76</v>
       </c>
       <c r="I46">
-        <v>708.65</v>
-      </c>
-      <c r="J46">
-        <v>792.4</v>
+        <v>9446.1</v>
       </c>
       <c r="K46" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L46">
-        <v>515.79999999999995</v>
+        <v>9105.75</v>
       </c>
       <c r="M46">
         <v>2</v>
       </c>
       <c r="N46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -2598,40 +2613,37 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <v>44477</v>
+        <v>44483</v>
       </c>
       <c r="D47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E47">
-        <v>97.75</v>
+        <v>358</v>
       </c>
       <c r="F47">
-        <v>90.97</v>
+        <v>327.27999999999997</v>
       </c>
       <c r="G47">
-        <v>88.12</v>
+        <v>321.62</v>
       </c>
       <c r="H47">
-        <v>102.15</v>
+        <v>374.11</v>
       </c>
       <c r="I47">
-        <v>106.95</v>
-      </c>
-      <c r="J47">
-        <v>122.7</v>
+        <v>377.57</v>
       </c>
       <c r="K47" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="L47">
-        <v>97.45</v>
+        <v>318.55</v>
       </c>
       <c r="M47">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="N47" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -2642,40 +2654,40 @@
         <v>1</v>
       </c>
       <c r="C48" s="1">
-        <v>44477</v>
+        <v>44482</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E48">
-        <v>1965.1</v>
+        <v>1840.1</v>
       </c>
       <c r="F48">
-        <v>1863.54</v>
+        <v>1728.38</v>
       </c>
       <c r="G48">
-        <v>1850.86</v>
+        <v>1649.84</v>
       </c>
       <c r="H48">
-        <v>2053.5300000000002</v>
+        <v>1922.9</v>
       </c>
       <c r="I48">
-        <v>2073.9699999999998</v>
+        <v>1954.85</v>
       </c>
       <c r="J48">
-        <v>2147.83</v>
+        <v>2179.75</v>
       </c>
       <c r="K48" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L48">
-        <v>1946.05</v>
+        <v>1792.45</v>
       </c>
       <c r="M48">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
@@ -2686,37 +2698,37 @@
         <v>1</v>
       </c>
       <c r="C49" s="1">
-        <v>44477</v>
+        <v>44481</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E49">
-        <v>211.55</v>
+        <v>456.35</v>
       </c>
       <c r="F49">
-        <v>199.66</v>
+        <v>431.76</v>
       </c>
       <c r="G49">
-        <v>195.14</v>
+        <v>421.61</v>
       </c>
       <c r="H49">
-        <v>221.07</v>
+        <v>476.89</v>
       </c>
       <c r="I49">
-        <v>222.5</v>
+        <v>476.9</v>
       </c>
       <c r="J49">
-        <v>231.5</v>
+        <v>531.9</v>
       </c>
       <c r="K49" t="s">
         <v>15</v>
       </c>
       <c r="L49">
-        <v>197.65</v>
+        <v>464.65</v>
       </c>
       <c r="M49">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N49" t="s">
         <v>4</v>
@@ -2730,37 +2742,40 @@
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <v>44476</v>
+        <v>44481</v>
       </c>
       <c r="D50" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E50">
-        <v>2141.3000000000002</v>
+        <v>96.3</v>
       </c>
       <c r="F50">
-        <v>1927.17</v>
+        <v>91.74</v>
       </c>
       <c r="G50">
-        <v>1897.63</v>
+        <v>88.31</v>
       </c>
       <c r="H50">
-        <v>2237.66</v>
+        <v>100.63</v>
       </c>
       <c r="I50">
-        <v>2357.87</v>
+        <v>106.95</v>
+      </c>
+      <c r="J50">
+        <v>122.7</v>
       </c>
       <c r="K50" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="L50">
-        <v>1949.45</v>
+        <v>102.55</v>
       </c>
       <c r="M50">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="N50" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -2771,31 +2786,34 @@
         <v>1</v>
       </c>
       <c r="C51" s="1">
-        <v>44476</v>
+        <v>44481</v>
       </c>
       <c r="D51" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E51">
-        <v>1304.5</v>
+        <v>2025</v>
       </c>
       <c r="F51">
-        <v>1181.8499999999999</v>
+        <v>1869.62</v>
       </c>
       <c r="G51">
-        <v>1177.8599999999999</v>
+        <v>1853.79</v>
       </c>
       <c r="H51">
-        <v>1357.02</v>
+        <v>2116.13</v>
       </c>
       <c r="I51">
-        <v>1363.2</v>
+        <v>2147.83</v>
+      </c>
+      <c r="J51">
+        <v>2419.38</v>
       </c>
       <c r="K51" t="s">
         <v>15</v>
       </c>
       <c r="L51">
-        <v>1313.25</v>
+        <v>1993.8</v>
       </c>
       <c r="M51">
         <v>2</v>
@@ -2812,34 +2830,37 @@
         <v>1</v>
       </c>
       <c r="C52" s="1">
-        <v>44476</v>
+        <v>44480</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E52">
-        <v>1046</v>
+        <v>313.55</v>
       </c>
       <c r="F52">
-        <v>991.55</v>
+        <v>297.8</v>
       </c>
       <c r="G52">
-        <v>975.33</v>
+        <v>282.27</v>
       </c>
       <c r="H52">
-        <v>1093.07</v>
+        <v>323.38</v>
       </c>
       <c r="I52">
-        <v>1100.17</v>
+        <v>327.66000000000003</v>
+      </c>
+      <c r="J52">
+        <v>334.27</v>
       </c>
       <c r="K52" t="s">
         <v>6</v>
       </c>
       <c r="L52">
-        <v>804.35</v>
+        <v>269.75</v>
       </c>
       <c r="M52">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N52" t="s">
         <v>6</v>
@@ -2853,40 +2874,40 @@
         <v>1</v>
       </c>
       <c r="C53" s="1">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="D53" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E53">
-        <v>310.7</v>
+        <v>789.25</v>
       </c>
       <c r="F53">
-        <v>295.52999999999997</v>
+        <v>757.08</v>
       </c>
       <c r="G53">
-        <v>280.48</v>
+        <v>751.14</v>
       </c>
       <c r="H53">
-        <v>323.38</v>
+        <v>816.23</v>
       </c>
       <c r="I53">
-        <v>324.68</v>
+        <v>824.77</v>
       </c>
       <c r="J53">
-        <v>334.27</v>
+        <v>834.78</v>
       </c>
       <c r="K53" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L53">
-        <v>273.3</v>
+        <v>821</v>
       </c>
       <c r="M53">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N53" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
@@ -2897,40 +2918,40 @@
         <v>1</v>
       </c>
       <c r="C54" s="1">
-        <v>44475</v>
+        <v>44477</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E54">
-        <v>214.3</v>
+        <v>656.4</v>
       </c>
       <c r="F54">
-        <v>206.45</v>
+        <v>653</v>
       </c>
       <c r="G54">
-        <v>205.8</v>
+        <v>632.46</v>
       </c>
       <c r="H54">
-        <v>223.94</v>
+        <v>685.94</v>
       </c>
       <c r="I54">
-        <v>225.65</v>
+        <v>708.65</v>
       </c>
       <c r="J54">
-        <v>245.35</v>
+        <v>792.4</v>
       </c>
       <c r="K54" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L54">
-        <v>214.4</v>
+        <v>515.79999999999995</v>
       </c>
       <c r="M54">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N54" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
@@ -2941,37 +2962,40 @@
         <v>1</v>
       </c>
       <c r="C55" s="1">
-        <v>44474</v>
+        <v>44477</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E55">
-        <v>289</v>
+        <v>97.75</v>
       </c>
       <c r="F55">
-        <v>276.52</v>
+        <v>90.97</v>
       </c>
       <c r="G55">
-        <v>272.33</v>
+        <v>88.12</v>
       </c>
       <c r="H55">
-        <v>302</v>
+        <v>102.15</v>
       </c>
       <c r="I55">
-        <v>306.18</v>
+        <v>106.95</v>
+      </c>
+      <c r="J55">
+        <v>122.7</v>
       </c>
       <c r="K55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L55">
+        <v>97.45</v>
+      </c>
+      <c r="M55">
         <v>15</v>
       </c>
-      <c r="L55">
-        <v>283.05</v>
-      </c>
-      <c r="M55">
-        <v>13</v>
-      </c>
       <c r="N55" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
@@ -2982,39 +3006,379 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
+        <v>44477</v>
+      </c>
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56">
+        <v>1965.1</v>
+      </c>
+      <c r="F56">
+        <v>1863.54</v>
+      </c>
+      <c r="G56">
+        <v>1850.86</v>
+      </c>
+      <c r="H56">
+        <v>2053.5300000000002</v>
+      </c>
+      <c r="I56">
+        <v>2073.9699999999998</v>
+      </c>
+      <c r="J56">
+        <v>2147.83</v>
+      </c>
+      <c r="K56" t="s">
+        <v>3</v>
+      </c>
+      <c r="L56">
+        <v>1946.05</v>
+      </c>
+      <c r="M56">
+        <v>4</v>
+      </c>
+      <c r="N56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44477</v>
+      </c>
+      <c r="D57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57">
+        <v>211.55</v>
+      </c>
+      <c r="F57">
+        <v>199.66</v>
+      </c>
+      <c r="G57">
+        <v>195.14</v>
+      </c>
+      <c r="H57">
+        <v>221.07</v>
+      </c>
+      <c r="I57">
+        <v>222.5</v>
+      </c>
+      <c r="J57">
+        <v>231.5</v>
+      </c>
+      <c r="K57" t="s">
+        <v>15</v>
+      </c>
+      <c r="L57">
+        <v>197.65</v>
+      </c>
+      <c r="M57">
+        <v>5</v>
+      </c>
+      <c r="N57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58">
+        <v>2141.3000000000002</v>
+      </c>
+      <c r="F58">
+        <v>1927.17</v>
+      </c>
+      <c r="G58">
+        <v>1897.63</v>
+      </c>
+      <c r="H58">
+        <v>2237.66</v>
+      </c>
+      <c r="I58">
+        <v>2357.87</v>
+      </c>
+      <c r="K58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L58">
+        <v>1949.45</v>
+      </c>
+      <c r="M58">
+        <v>15</v>
+      </c>
+      <c r="N58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59">
+        <v>1304.5</v>
+      </c>
+      <c r="F59">
+        <v>1181.8499999999999</v>
+      </c>
+      <c r="G59">
+        <v>1177.8599999999999</v>
+      </c>
+      <c r="H59">
+        <v>1357.02</v>
+      </c>
+      <c r="I59">
+        <v>1363.2</v>
+      </c>
+      <c r="K59" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59">
+        <v>1313.25</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="N59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D60" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60">
+        <v>1046</v>
+      </c>
+      <c r="F60">
+        <v>991.55</v>
+      </c>
+      <c r="G60">
+        <v>975.33</v>
+      </c>
+      <c r="H60">
+        <v>1093.07</v>
+      </c>
+      <c r="I60">
+        <v>1100.17</v>
+      </c>
+      <c r="K60" t="s">
+        <v>6</v>
+      </c>
+      <c r="L60">
+        <v>804.35</v>
+      </c>
+      <c r="M60">
+        <v>4</v>
+      </c>
+      <c r="N60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>44476</v>
+      </c>
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61">
+        <v>310.7</v>
+      </c>
+      <c r="F61">
+        <v>295.52999999999997</v>
+      </c>
+      <c r="G61">
+        <v>280.48</v>
+      </c>
+      <c r="H61">
+        <v>323.38</v>
+      </c>
+      <c r="I61">
+        <v>324.68</v>
+      </c>
+      <c r="J61">
+        <v>334.27</v>
+      </c>
+      <c r="K61" t="s">
+        <v>6</v>
+      </c>
+      <c r="L61">
+        <v>273.3</v>
+      </c>
+      <c r="M61">
+        <v>9</v>
+      </c>
+      <c r="N61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>44475</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>214.3</v>
+      </c>
+      <c r="F62">
+        <v>206.45</v>
+      </c>
+      <c r="G62">
+        <v>205.8</v>
+      </c>
+      <c r="H62">
+        <v>223.94</v>
+      </c>
+      <c r="I62">
+        <v>225.65</v>
+      </c>
+      <c r="J62">
+        <v>245.35</v>
+      </c>
+      <c r="K62" t="s">
+        <v>3</v>
+      </c>
+      <c r="L62">
+        <v>214.4</v>
+      </c>
+      <c r="M62">
+        <v>9</v>
+      </c>
+      <c r="N62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44474</v>
+      </c>
+      <c r="D63" t="s">
+        <v>55</v>
+      </c>
+      <c r="E63">
+        <v>289</v>
+      </c>
+      <c r="F63">
+        <v>276.52</v>
+      </c>
+      <c r="G63">
+        <v>272.33</v>
+      </c>
+      <c r="H63">
+        <v>302</v>
+      </c>
+      <c r="I63">
+        <v>306.18</v>
+      </c>
+      <c r="K63" t="s">
+        <v>15</v>
+      </c>
+      <c r="L63">
+        <v>283.05</v>
+      </c>
+      <c r="M63">
+        <v>13</v>
+      </c>
+      <c r="N63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1">
         <v>44470</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D64" t="s">
         <v>56</v>
       </c>
-      <c r="E56">
+      <c r="E64">
         <v>3396.6</v>
       </c>
-      <c r="F56">
+      <c r="F64">
         <v>3162.72</v>
       </c>
-      <c r="G56">
+      <c r="G64">
         <v>3027.58</v>
       </c>
-      <c r="H56">
+      <c r="H64">
         <v>3549.45</v>
       </c>
-      <c r="I56">
+      <c r="I64">
         <v>3557.23</v>
       </c>
-      <c r="J56">
+      <c r="J64">
         <v>3951.23</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K64" t="s">
         <v>15</v>
       </c>
-      <c r="L56">
+      <c r="L64">
         <v>3392.4</v>
       </c>
-      <c r="M56">
+      <c r="M64">
         <v>7</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N64" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>